<commit_message>
se modifico y añadio video
</commit_message>
<xml_diff>
--- a/Version Datos-1/Ingredientes.xlsx
+++ b/Version Datos-1/Ingredientes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseg\Documents\GitHub\OOPProyectFinal\Version Datos-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C2642B-3CF7-41D9-B12E-0C8E171C3727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F83E2CE-3D45-42E7-814B-DA4B8079A608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B06623A7-46AA-4AFB-AE9C-D78C0EB063C3}"/>
+    <workbookView xWindow="7572" yWindow="420" windowWidth="10896" windowHeight="11496" xr2:uid="{B06623A7-46AA-4AFB-AE9C-D78C0EB063C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Precio</t>
   </si>
@@ -63,6 +63,36 @@
   </si>
   <si>
     <t>Stock</t>
+  </si>
+  <si>
+    <t>Carne de Res</t>
+  </si>
+  <si>
+    <t>Carne de Pollo</t>
+  </si>
+  <si>
+    <t>Mixta</t>
+  </si>
+  <si>
+    <t>Pan Integral</t>
+  </si>
+  <si>
+    <t>Pan Blanco</t>
+  </si>
+  <si>
+    <t>Pan de Oregano</t>
+  </si>
+  <si>
+    <t>Mayonesa</t>
+  </si>
+  <si>
+    <t>Ketchup</t>
+  </si>
+  <si>
+    <t>Piña</t>
+  </si>
+  <si>
+    <t>Cebolla Dulce</t>
   </si>
 </sst>
 </file>
@@ -414,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865E0581-0AEA-49AA-B47A-E0D4E2368305}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -435,10 +465,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>8000</v>
       </c>
       <c r="C2">
         <v>20</v>
@@ -446,10 +476,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>7000</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -457,10 +487,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B4">
-        <v>150</v>
+        <v>10000</v>
       </c>
       <c r="C4">
         <v>20</v>
@@ -468,10 +498,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B5">
-        <v>200</v>
+        <v>2000</v>
       </c>
       <c r="C5">
         <v>20</v>
@@ -479,10 +509,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B6">
-        <v>100</v>
+        <v>2000</v>
       </c>
       <c r="C6">
         <v>20</v>
@@ -490,12 +520,122 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>2000</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>150</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>200</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B13">
         <v>150</v>
       </c>
-      <c r="C7">
+      <c r="C13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>200</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>200</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>200</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>200</v>
+      </c>
+      <c r="C17">
         <v>20</v>
       </c>
     </row>

</xml_diff>